<commit_message>
Compiled exo/endo mapped reads and organized
</commit_message>
<xml_diff>
--- a/eCAMI/mapped_reads_all.xlsx
+++ b/eCAMI/mapped_reads_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/CRDS_Calcs/eCAMI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{EAC8F5B1-9C7A-4D3E-8FA0-65E395083545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{883EFAAB-6162-4DDB-A954-9DF3C215BCC4}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{EAC8F5B1-9C7A-4D3E-8FA0-65E395083545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F3779AC-52A1-47C0-AD08-49C3572688AA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BADEA35-55E2-4862-8C07-FC655D6CC413}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
   <si>
     <t>Sample</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>RelAbund*100000</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Winter</t>
   </si>
 </sst>
 </file>
@@ -475,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A7045B-F6B7-4D9F-922A-633B7CAD8682}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +498,7 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,8 +517,11 @@
       <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -526,8 +541,11 @@
         <f>(D2/E2)*100000</f>
         <v>2.0830489392906496E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -547,8 +565,11 @@
         <f t="shared" ref="F3:F28" si="0">(D3/E3)*100000</f>
         <v>4.1905179160617256E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -568,8 +589,11 @@
         <f t="shared" si="0"/>
         <v>2.3761193541859669E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -589,8 +613,11 @@
         <f t="shared" si="0"/>
         <v>0.50169998931425908</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -610,8 +637,11 @@
         <f t="shared" si="0"/>
         <v>1.425177998318689E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -632,8 +662,11 @@
         <f t="shared" si="0"/>
         <v>2.4117077719342856</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -654,8 +687,11 @@
         <f t="shared" si="0"/>
         <v>4.4550443595131224</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -676,8 +712,11 @@
         <f t="shared" si="0"/>
         <v>3.6650355434008515</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -698,8 +737,11 @@
         <f t="shared" si="0"/>
         <v>4.2532536439928803</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -720,8 +762,11 @@
         <f t="shared" si="0"/>
         <v>6.2141105913294155</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -742,8 +787,11 @@
         <f t="shared" si="0"/>
         <v>1.5730873496722799</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -764,8 +812,11 @@
         <f t="shared" si="0"/>
         <v>7.8308647910752853</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -786,8 +837,11 @@
         <f t="shared" si="0"/>
         <v>4.1544113330122192</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -808,8 +862,11 @@
         <f t="shared" si="0"/>
         <v>1.4337290663086011</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -829,8 +886,11 @@
         <f t="shared" si="0"/>
         <v>5.2477857253337701E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -850,8 +910,11 @@
         <f t="shared" si="0"/>
         <v>1.7481101880001605E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -871,8 +934,11 @@
         <f t="shared" si="0"/>
         <v>1.118399328985966E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -892,8 +958,11 @@
         <f t="shared" si="0"/>
         <v>1.6059304312864283E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -914,8 +983,11 @@
         <f t="shared" si="0"/>
         <v>5.59231426643177</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -936,8 +1008,11 @@
         <f t="shared" si="0"/>
         <v>4.0905778399203756</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -958,8 +1033,11 @@
         <f t="shared" si="0"/>
         <v>5.9306154104228082</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -980,8 +1058,11 @@
         <f t="shared" si="0"/>
         <v>1.7335189599282474</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1002,8 +1083,11 @@
         <f t="shared" si="0"/>
         <v>5.7343556599011878</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1024,8 +1108,11 @@
         <f t="shared" si="0"/>
         <v>7.4985037186383332</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1046,8 +1133,11 @@
         <f t="shared" si="0"/>
         <v>16.756769459853256</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1068,8 +1158,11 @@
         <f t="shared" si="0"/>
         <v>4.7021643028066622</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1089,6 +1182,9 @@
       <c r="F28">
         <f t="shared" si="0"/>
         <v>4.183136457053819</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to inulinase files
</commit_message>
<xml_diff>
--- a/eCAMI/mapped_reads_all.xlsx
+++ b/eCAMI/mapped_reads_all.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="139" documentId="8_{EAC8F5B1-9C7A-4D3E-8FA0-65E395083545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{255A1E74-6263-42C6-A40B-BED941998896}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3BADEA35-55E2-4862-8C07-FC655D6CC413}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BADEA35-55E2-4862-8C07-FC655D6CC413}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,16 +498,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A7045B-F6B7-4D9F-922A-633B7CAD8682}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -560,7 +560,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -587,7 +587,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -614,7 +614,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -641,7 +641,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -668,7 +668,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -696,7 +696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -724,7 +724,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -752,7 +752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -780,7 +780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -808,7 +808,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -836,7 +836,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -864,7 +864,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -892,7 +892,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -920,7 +920,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -947,7 +947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -974,7 +974,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>

</xml_diff>